<commit_message>
Abre site e pesquisa produto
</commit_message>
<xml_diff>
--- a/consultaPrecos/produtos.xlsx
+++ b/consultaPrecos/produtos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbf25413570eb110/Documents/GitHub/consultaPrecos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbf25413570eb110/Documents/GitHub/atualiza_precos/consultaPrecos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_AD4D361C20488DEA4E38A0734CDB543E5ADEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DDED545-CF18-401A-9374-03C1F0771AD6}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_AD4D361C20488DEA4E38A0734CDB543E5ADEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A16695EB-D2D2-4A52-B32E-23AB71FEBAC6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,13 +30,13 @@
     <t>Produtos</t>
   </si>
   <si>
-    <t>Precos</t>
-  </si>
-  <si>
     <t>Monitor LG UltraWide™ LG 29'' Full HD IPS HDR10 - 29WK600-W</t>
   </si>
   <si>
     <t>Mouse Gamer Razer Deathadder V2 Mini</t>
+  </si>
+  <si>
+    <t>Preços/data</t>
   </si>
 </sst>
 </file>
@@ -97,6 +97,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -362,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -379,17 +383,20 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>